<commit_message>
Adding GUI text interface
</commit_message>
<xml_diff>
--- a/matching_results Sundar Pichai.xlsx
+++ b/matching_results Sundar Pichai.xlsx
@@ -448,61 +448,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mark zuckerberg.jpeg</t>
+          <t>Sundar Pichai 1.jpg</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>satya nadella 2.jpeg</t>
+          <t>Mark 6.png</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>522</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mark 6.png</t>
+          <t>Mark3.png</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1180</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sundar Pichai 1.jpg</t>
+          <t>Sundar Pichai 3.png</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1368</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mark3.png</t>
+          <t>satya nadella 2.jpeg</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1602</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sundar Pichai 3.png</t>
+          <t>mark zuckerberg.jpeg</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2128</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2814</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="9">
@@ -522,27 +522,27 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3476</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>satya nadella 2.png</t>
+          <t>Mark2.jpg</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4184</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mark2.jpg</t>
+          <t>satya nadella 2.png</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4862</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>158169</v>
+        <v>115087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Image displayed in GUI
</commit_message>
<xml_diff>
--- a/matching_results Sundar Pichai.xlsx
+++ b/matching_results Sundar Pichai.xlsx
@@ -448,61 +448,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Sundar Pichai 1.jpg</t>
+          <t>mark zuckerberg.jpeg</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Mark 6.png</t>
+          <t>satya nadella 2.jpeg</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>300</v>
+        <v>522</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mark3.png</t>
+          <t>Mark 6.png</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>542</v>
+        <v>1180</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sundar Pichai 3.png</t>
+          <t>Sundar Pichai 1.jpg</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1112</v>
+        <v>1368</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>satya nadella 2.jpeg</t>
+          <t>Mark3.png</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1230</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>mark zuckerberg.jpeg</t>
+          <t>Sundar Pichai 3.png</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>1364</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>1446</v>
+        <v>2814</v>
       </c>
     </row>
     <row r="9">
@@ -522,27 +522,27 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>2108</v>
+        <v>3476</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Mark2.jpg</t>
+          <t>satya nadella 2.png</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>3494</v>
+        <v>4184</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>satya nadella 2.png</t>
+          <t>Mark2.jpg</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4450</v>
+        <v>4862</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>115087</v>
+        <v>158169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added info about the project
</commit_message>
<xml_diff>
--- a/matching_results Sundar Pichai.xlsx
+++ b/matching_results Sundar Pichai.xlsx
@@ -448,61 +448,61 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>mark zuckerberg.jpeg</t>
+          <t>Sundar Pichai 1.jpg</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>96</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>satya nadella 2.jpeg</t>
+          <t>Mark 6.png</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>522</v>
+        <v>300</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Mark 6.png</t>
+          <t>Mark3.png</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>1180</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sundar Pichai 1.jpg</t>
+          <t>Sundar Pichai 3.png</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>1368</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Mark3.png</t>
+          <t>satya nadella 2.jpeg</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>1602</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Sundar Pichai 3.png</t>
+          <t>mark zuckerberg.jpeg</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2128</v>
+        <v>1364</v>
       </c>
     </row>
     <row r="8">
@@ -512,7 +512,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>2814</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="9">
@@ -522,27 +522,27 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>3476</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>satya nadella 2.png</t>
+          <t>Mark2.jpg</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>4184</v>
+        <v>3494</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Mark2.jpg</t>
+          <t>satya nadella 2.png</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>4862</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="12">
@@ -552,7 +552,7 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>158169</v>
+        <v>115087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>